<commit_message>
14.1 Validaciones - Botones - Colores - Plantilla
</commit_message>
<xml_diff>
--- a/servidor/plantillasVacias/Empleados.xlsx
+++ b/servidor/plantillasVacias/Empleados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jennytipan\Desktop\ProyectoFulltime\FullTimeV3\servidor\plantillasVacias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F50DE2D-3E61-47F2-8B14-119969A11BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C791A6-9018-4A62-A749-574A4BBF4F04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="387">
   <si>
     <t>apellido</t>
   </si>
@@ -1187,12 +1187,6 @@
   </si>
   <si>
     <t>nacionalidad</t>
-  </si>
-  <si>
-    <t>codigo</t>
-  </si>
-  <si>
-    <t>1756987457</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1285,9 +1279,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1571,172 +1562,165 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>387</v>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>5</v>
+        <v>386</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>386</v>
+        <v>6</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="R1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>388</v>
+      <c r="B2" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="H2" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="I2" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="L2" s="3" t="s">
+        <v>131</v>
+      </c>
       <c r="M2" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="N2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="4">
+      <c r="N2" s="4">
         <v>12345</v>
       </c>
-      <c r="P2" s="3" t="b">
+      <c r="O2" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="R2" s="3" t="b">
+      <c r="Q2" s="3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="O3" s="4"/>
-    </row>
-    <row r="4" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="O4" s="4"/>
-    </row>
-    <row r="5" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="5"/>
-      <c r="H5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="O5" s="4"/>
-    </row>
-    <row r="6" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G6" s="4"/>
+    <row r="3" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="5"/>
+      <c r="G3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="5"/>
+      <c r="G4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="5"/>
+      <c r="G5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F6" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{D0D17A7E-B2D2-48F3-97A4-EF405D78F5C7}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{D0D17A7E-B2D2-48F3-97A4-EF405D78F5C7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
@@ -1747,31 +1731,31 @@
           <x14:formula1>
             <xm:f>Selectores!$B$2:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E5517</xm:sqref>
+          <xm:sqref>D2:D5517</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{81EF18B1-CCC1-448F-98BE-DBCBFB4C7686}">
           <x14:formula1>
             <xm:f>Selectores!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F6031</xm:sqref>
+          <xm:sqref>E2:E6031</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6E9A3189-0EFB-45FA-8035-BD512385254B}">
           <x14:formula1>
             <xm:f>Selectores!$F$2:$F$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I6031</xm:sqref>
+          <xm:sqref>H2:H6031</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{83249B3F-4CFF-4C26-8DEE-1F14503326E0}">
           <x14:formula1>
             <xm:f>Selectores!$H$2:$H$347</xm:f>
           </x14:formula1>
-          <xm:sqref>M2:M6965</xm:sqref>
+          <xm:sqref>L2:L6965</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F6A31D00-3FD0-4626-ABD1-A71C138045F1}">
           <x14:formula1>
             <xm:f>Selectores!$J$2:$J$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P6828 R2:R6083</xm:sqref>
+          <xm:sqref>O2:O6828 Q2:Q6083</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>